<commit_message>
Create simple CRUD of Zuper
</commit_message>
<xml_diff>
--- a/.dev/zuper_registers.xlsx
+++ b/.dev/zuper_registers.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -53,12 +55,31 @@
   </si>
   <si>
     <t>Rua Logo Ali, 33</t>
+  </si>
+  <si>
+    <t>Xablau</t>
+  </si>
+  <si>
+    <t>Ali na esquena 123</t>
+  </si>
+  <si>
+    <t>12978465</t>
+  </si>
+  <si>
+    <t>Logo Ali 123</t>
+  </si>
+  <si>
+    <t>Logo Ali 123478457</t>
+  </si>
+  <si>
+    <t>teste</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -304,6 +325,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -393,6 +415,48 @@
         <v>2042030.0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>796.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>212.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>686.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>